<commit_message>
remove crowpasstrail from sde_common
</commit_message>
<xml_diff>
--- a/data/Y_inventory_working.xlsx
+++ b/data/Y_inventory_working.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\updateDataSources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F264D34-36BC-4561-875D-249B736E4649}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556EF6EF-5CE7-46F9-AF32-472B68BC08EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CA5E6435-CCC8-4325-8D7B-F96E7D205BA8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$223</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$222</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="285">
   <si>
     <t>Y:\sde_wcgis_master (dfgjnusql-gi71p).sde\sde_wcgis_master.DBO.areanamesCurrent</t>
   </si>
@@ -823,12 +823,6 @@
   </si>
   <si>
     <t>Y:\sde_common (dfgjnusql-gi71p).sde\sde_common.DBO.BaseFeatures\sde_common.DBO.Chugach_SP_Trails</t>
-  </si>
-  <si>
-    <t>Y:\sde_common (dfgjnusql-gi71p).sde\sde_common.DBO.BaseFeatures\sde_common.DBO.crowpasstrail</t>
-  </si>
-  <si>
-    <t>crowpasstrail</t>
   </si>
   <si>
     <t>Y:\sde_common (dfgjnusql-gi71p).sde\sde_common.DBO.BaseFeatures\sde_common.DBO.dudded_impact_area</t>
@@ -1267,12 +1261,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1839E316-BE17-4D06-9A89-F663D4A5EC12}">
-  <dimension ref="A1:G223"/>
+  <dimension ref="A1:G222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="A216" sqref="A216:XFD216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5227,7 +5221,7 @@
         <v>241</v>
       </c>
       <c r="C204" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>220</v>
@@ -5251,7 +5245,7 @@
         <v>242</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>220</v>
@@ -5299,7 +5293,7 @@
         <v>243</v>
       </c>
       <c r="C207" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>220</v>
@@ -5323,7 +5317,7 @@
         <v>244</v>
       </c>
       <c r="C208" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>220</v>
@@ -5344,7 +5338,7 @@
         <v>245</v>
       </c>
       <c r="C209" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>220</v>
@@ -5365,7 +5359,7 @@
         <v>246</v>
       </c>
       <c r="C210" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>220</v>
@@ -5389,7 +5383,7 @@
         <v>247</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>220</v>
@@ -5410,7 +5404,7 @@
         <v>248</v>
       </c>
       <c r="C212" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>220</v>
@@ -5434,7 +5428,7 @@
         <v>249</v>
       </c>
       <c r="C213" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>220</v>
@@ -5464,7 +5458,7 @@
         <v>220</v>
       </c>
       <c r="E214" t="str">
-        <f t="shared" ref="E214:E221" si="7">IF(ISERROR(FIND("\",C214)),C214,RIGHT(C214,LEN(C214)-
+        <f t="shared" ref="E214:E220" si="7">IF(ISERROR(FIND("\",C214)),C214,RIGHT(C214,LEN(C214)-
 FIND("~",SUBSTITUTE(C214,"\","~",LEN(C214)-LEN(SUBSTITUTE(C214,"\",""))))))</f>
         <v>sde_common.DBO.Chugach_NF_Trails</v>
       </c>
@@ -5501,20 +5495,20 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C216" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>220</v>
       </c>
       <c r="E216" t="str">
         <f t="shared" si="7"/>
-        <v>sde_common.DBO.crowpasstrail</v>
+        <v>sde_common.DBO.railroad</v>
       </c>
       <c r="F216" t="s">
         <v>251</v>
@@ -5525,7 +5519,7 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>267</v>
@@ -5538,7 +5532,7 @@
       </c>
       <c r="E217" t="str">
         <f t="shared" si="7"/>
-        <v>sde_common.DBO.railroad</v>
+        <v>sde_common.DBO.rextrail</v>
       </c>
       <c r="F217" t="s">
         <v>251</v>
@@ -5549,7 +5543,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>269</v>
@@ -5562,7 +5556,7 @@
       </c>
       <c r="E218" t="str">
         <f t="shared" si="7"/>
-        <v>sde_common.DBO.rextrail</v>
+        <v>sde_common.DBO.RS2477_Trails</v>
       </c>
       <c r="F218" t="s">
         <v>251</v>
@@ -5573,20 +5567,20 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>271</v>
       </c>
       <c r="C219" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>220</v>
       </c>
       <c r="E219" t="str">
         <f t="shared" si="7"/>
-        <v>sde_common.DBO.RS2477_Trails</v>
+        <v>sde_common.DBO.Legislatively_Designated_Area_Py</v>
       </c>
       <c r="F219" t="s">
         <v>251</v>
@@ -5597,20 +5591,20 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C220" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>220</v>
       </c>
       <c r="E220" t="str">
         <f t="shared" si="7"/>
-        <v>sde_common.DBO.Legislatively_Designated_Area_Py</v>
+        <v>sde_common.DBO.NPS_Boundary</v>
       </c>
       <c r="F220" t="s">
         <v>251</v>
@@ -5621,20 +5615,21 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C221" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>220</v>
       </c>
       <c r="E221" t="str">
-        <f t="shared" si="7"/>
-        <v>sde_common.DBO.NPS_Boundary</v>
+        <f t="shared" ref="E221:E222" si="8">IF(ISERROR(FIND("\",C221)),C221,RIGHT(C221,LEN(C221)-
+FIND("~",SUBSTITUTE(C221,"\","~",LEN(C221)-LEN(SUBSTITUTE(C221,"\",""))))))</f>
+        <v>sde_common.DBO.AK_coast_250K</v>
       </c>
       <c r="F221" t="s">
         <v>251</v>
@@ -5645,21 +5640,20 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C222" t="s">
         <v>275</v>
       </c>
-      <c r="C222" t="s">
-        <v>280</v>
-      </c>
       <c r="D222" s="2" t="s">
         <v>220</v>
       </c>
       <c r="E222" t="str">
-        <f t="shared" ref="E222:E223" si="8">IF(ISERROR(FIND("\",C222)),C222,RIGHT(C222,LEN(C222)-
-FIND("~",SUBSTITUTE(C222,"\","~",LEN(C222)-LEN(SUBSTITUTE(C222,"\",""))))))</f>
-        <v>sde_common.DBO.AK_coast_250K</v>
+        <f t="shared" si="8"/>
+        <v>sde_common.DBO.ADFG_logo_2001_transparent</v>
       </c>
       <c r="F222" t="s">
         <v>251</v>
@@ -5668,34 +5662,10 @@
         <v>257</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A223" s="1">
-        <v>231</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C223" t="s">
-        <v>277</v>
-      </c>
-      <c r="D223" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E223" t="str">
-        <f t="shared" si="8"/>
-        <v>sde_common.DBO.ADFG_logo_2001_transparent</v>
-      </c>
-      <c r="F223" t="s">
-        <v>251</v>
-      </c>
-      <c r="G223" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F223" xr:uid="{E3DA9AB2-34A2-4E46-B8BF-4D56B82CD0F8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F216">
-      <sortCondition ref="A1:A216"/>
+  <autoFilter ref="A1:F222" xr:uid="{E3DA9AB2-34A2-4E46-B8BF-4D56B82CD0F8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F215">
+      <sortCondition ref="A1:A215"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>